<commit_message>
Bug fix: for #4
the mode of vim was not registerd propely
</commit_message>
<xml_diff>
--- a/sys_plugin/vim/data/register.xlsx
+++ b/sys_plugin/vim/data/register.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koji0\Desktop\ExcelLikeVim\sys_plugin\vim\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB52E86-21AC-484F-AEFF-BFB6A4E7DF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="480" yWindow="120" windowWidth="18240" windowHeight="8505"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -32,65 +38,17 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>列幅</t>
-    <rPh sb="0" eb="2">
-      <t>レツハバ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1:16384</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>line_visual</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MPM入力の進行</t>
-    <rPh sb="3" eb="5">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シンコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>全体ワークフロー作成</t>
-    <rPh sb="0" eb="2">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>サクセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>たたき台完成</t>
-    <rPh sb="3" eb="4">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>カンセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タウン</t>
-    <phoneticPr fontId="1"/>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;\ \(aaa\)"/>
-    <numFmt numFmtId="178" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -102,27 +60,6 @@
       <sz val="6"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial Unicode MS"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <name val="Arial Unicode MS"/>
-      <family val="3"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -143,56 +80,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -223,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -265,7 +167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -298,9 +200,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,6 +252,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,17 +444,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,85 +467,32 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:24" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="6">
-        <v>42236</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8">
-        <v>7</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="10">
-        <v>42236</v>
-      </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="8"/>
-    </row>
-    <row r="5" spans="1:24" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:24" ht="129" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:24" ht="128.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:24" ht="74.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:24" ht="71.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:24" ht="65.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:24" ht="129" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" ht="36.75" customHeight="1"/>
+    <row r="5" spans="1:4" ht="129" customHeight="1"/>
+    <row r="6" spans="1:4" ht="128.25" customHeight="1"/>
+    <row r="7" spans="1:4" ht="74.25" customHeight="1"/>
+    <row r="8" spans="1:4" ht="56.25" customHeight="1"/>
+    <row r="9" spans="1:4" ht="71.25" customHeight="1"/>
+    <row r="10" spans="1:4" ht="46.5" customHeight="1"/>
+    <row r="11" spans="1:4" ht="65.25" customHeight="1"/>
+    <row r="12" spans="1:4" ht="46.5" customHeight="1"/>
+    <row r="13" spans="1:4" ht="75" customHeight="1"/>
+    <row r="14" spans="1:4" ht="129" customHeight="1"/>
+    <row r="15" spans="1:4" ht="44.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="L4">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>L4=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>J4=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fix of unite link: when there is no link
</commit_message>
<xml_diff>
--- a/sys_plugin/vim/data/register.xlsx
+++ b/sys_plugin/vim/data/register.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koji0\Desktop\ExcelLikeVim\sys_plugin\vim\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watkoji\Desktop\ExcelLikeVim\sys_plugin\vim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB52E86-21AC-484F-AEFF-BFB6A4E7DF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCE0A2A-6231-42CA-9714-B3136FE3D587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -94,24 +105,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,7 +121,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,7 +448,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">

</xml_diff>